<commit_message>
The stock program are totaly usefull
</commit_message>
<xml_diff>
--- a/Base de datos de stock.xlsx
+++ b/Base de datos de stock.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,35 +440,55 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.3</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>code</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>product</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>inventary</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>cost</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>benefit</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>date</t>
         </is>
@@ -481,24 +501,36 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Alfajor Fantoche</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="H2" t="n">
         <v>20</v>
       </c>
-      <c r="E2" t="n">
+      <c r="I2" t="n">
         <v>53</v>
       </c>
-      <c r="F2" t="n">
+      <c r="J2" t="n">
         <v>17</v>
       </c>
-      <c r="G2" t="n">
+      <c r="K2" t="n">
         <v>70</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="L2" s="2" t="n">
         <v>44785</v>
       </c>
     </row>
@@ -509,24 +541,36 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>Té "La Virginia"</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="H3" t="n">
         <v>209</v>
       </c>
-      <c r="E3" t="n">
+      <c r="I3" t="n">
         <v>7.7</v>
       </c>
-      <c r="F3" t="n">
+      <c r="J3" t="n">
         <v>2.3</v>
       </c>
-      <c r="G3" t="n">
+      <c r="K3" t="n">
         <v>10</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="L3" s="2" t="n">
         <v>44988</v>
       </c>
     </row>
@@ -537,24 +581,36 @@
       <c r="B4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>Té "Rosamonte"</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="H4" t="n">
         <v>6</v>
       </c>
-      <c r="E4" t="n">
+      <c r="I4" t="n">
         <v>7.7</v>
       </c>
-      <c r="F4" t="n">
+      <c r="J4" t="n">
         <v>2.3</v>
       </c>
-      <c r="G4" t="n">
+      <c r="K4" t="n">
         <v>10</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="L4" s="2" t="n">
         <v>45112</v>
       </c>
     </row>
@@ -565,24 +621,36 @@
       <c r="B5" t="n">
         <v>3</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>Mate cocido "El Litoral"</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="H5" t="n">
         <v>10</v>
       </c>
-      <c r="E5" t="n">
+      <c r="I5" t="n">
         <v>3.85</v>
       </c>
-      <c r="F5" t="n">
+      <c r="J5" t="n">
         <v>1.15</v>
       </c>
-      <c r="G5" t="n">
+      <c r="K5" t="n">
         <v>5</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="L5" s="2" t="n">
         <v>45050</v>
       </c>
     </row>
@@ -593,24 +661,36 @@
       <c r="B6" t="n">
         <v>4</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>Galletitas "Mediatarde"</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="H6" t="n">
         <v>5</v>
       </c>
-      <c r="E6" t="n">
+      <c r="I6" t="n">
         <v>76.92307692307692</v>
       </c>
-      <c r="F6" t="n">
+      <c r="J6" t="n">
         <v>23.07692307692308</v>
       </c>
-      <c r="G6" t="n">
+      <c r="K6" t="n">
         <v>100</v>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="L6" s="2" t="n">
         <v>45337</v>
       </c>
     </row>
@@ -621,24 +701,36 @@
       <c r="B7" t="n">
         <v>5</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>Leche "Ilolay"</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="H7" t="n">
         <v>6</v>
       </c>
-      <c r="E7" t="n">
+      <c r="I7" t="n">
         <v>100</v>
       </c>
-      <c r="F7" t="n">
+      <c r="J7" t="n">
         <v>30</v>
       </c>
-      <c r="G7" t="n">
+      <c r="K7" t="n">
         <v>130</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="L7" s="2" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -649,24 +741,36 @@
       <c r="B8" t="n">
         <v>6</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" t="n">
+        <v>6</v>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>Yerba "Playadito"</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="H8" t="n">
         <v>1</v>
       </c>
-      <c r="E8" t="n">
+      <c r="I8" t="n">
         <v>230.75</v>
       </c>
-      <c r="F8" t="n">
+      <c r="J8" t="n">
         <v>69.25</v>
       </c>
-      <c r="G8" t="n">
+      <c r="K8" t="n">
         <v>300</v>
       </c>
-      <c r="H8" s="2" t="n">
+      <c r="L8" s="2" t="n">
         <v>45427</v>
       </c>
     </row>
@@ -677,24 +781,36 @@
       <c r="B9" t="n">
         <v>7</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="n">
+        <v>7</v>
+      </c>
+      <c r="F9" t="n">
+        <v>7</v>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>Galletitas "Bananitas"</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="H9" t="n">
         <v>4</v>
       </c>
-      <c r="E9" t="n">
+      <c r="I9" t="n">
         <v>100</v>
       </c>
-      <c r="F9" t="n">
+      <c r="J9" t="n">
         <v>30</v>
       </c>
-      <c r="G9" t="n">
+      <c r="K9" t="n">
         <v>130</v>
       </c>
-      <c r="H9" s="2" t="n">
+      <c r="L9" s="2" t="n">
         <v>44908</v>
       </c>
     </row>
@@ -705,24 +821,36 @@
       <c r="B10" t="n">
         <v>8</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>Galletitas "Diversión"</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="H10" t="n">
         <v>5</v>
       </c>
-      <c r="E10" t="n">
+      <c r="I10" t="n">
         <v>123.08</v>
       </c>
-      <c r="F10" t="n">
+      <c r="J10" t="n">
         <v>36.92</v>
       </c>
-      <c r="G10" t="n">
+      <c r="K10" t="n">
         <v>160</v>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="L10" s="2" t="n">
         <v>44818</v>
       </c>
     </row>
@@ -733,24 +861,36 @@
       <c r="B11" t="n">
         <v>9</v>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="n">
+        <v>9</v>
+      </c>
+      <c r="F11" t="n">
+        <v>9</v>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>Galletitas "Vainillas"</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="H11" t="n">
         <v>4</v>
       </c>
-      <c r="E11" t="n">
+      <c r="I11" t="n">
         <v>38.46</v>
       </c>
-      <c r="F11" t="n">
+      <c r="J11" t="n">
         <v>11.54</v>
       </c>
-      <c r="G11" t="n">
+      <c r="K11" t="n">
         <v>50</v>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="L11" s="2" t="n">
         <v>45023</v>
       </c>
     </row>
@@ -761,24 +901,36 @@
       <c r="B12" t="n">
         <v>10</v>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>Galletitas "Miel"</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="H12" t="n">
         <v>1</v>
       </c>
-      <c r="E12" t="n">
+      <c r="I12" t="n">
         <v>76.92</v>
       </c>
-      <c r="F12" t="n">
+      <c r="J12" t="n">
         <v>23.08</v>
       </c>
-      <c r="G12" t="n">
+      <c r="K12" t="n">
         <v>100</v>
       </c>
-      <c r="H12" s="2" t="n">
+      <c r="L12" s="2" t="n">
         <v>44998</v>
       </c>
     </row>
@@ -789,24 +941,36 @@
       <c r="B13" t="n">
         <v>11</v>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" t="n">
+        <v>11</v>
+      </c>
+      <c r="F13" t="n">
+        <v>11</v>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>Galletitas "Pitusas"</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="H13" t="n">
         <v>6</v>
       </c>
-      <c r="E13" t="n">
+      <c r="I13" t="n">
         <v>53.85</v>
       </c>
-      <c r="F13" t="n">
+      <c r="J13" t="n">
         <v>16.15</v>
       </c>
-      <c r="G13" t="n">
+      <c r="K13" t="n">
         <v>70</v>
       </c>
-      <c r="H13" s="2" t="n">
+      <c r="L13" s="2" t="n">
         <v>44874</v>
       </c>
     </row>
@@ -817,24 +981,36 @@
       <c r="B14" t="n">
         <v>12</v>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" t="n">
+        <v>12</v>
+      </c>
+      <c r="E14" t="n">
+        <v>12</v>
+      </c>
+      <c r="F14" t="n">
+        <v>12</v>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>Galletitas "Fauna"</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="H14" t="n">
         <v>3</v>
       </c>
-      <c r="E14" t="n">
+      <c r="I14" t="n">
         <v>46.15</v>
       </c>
-      <c r="F14" t="n">
+      <c r="J14" t="n">
         <v>13.85</v>
       </c>
-      <c r="G14" t="n">
+      <c r="K14" t="n">
         <v>60</v>
       </c>
-      <c r="H14" s="2" t="n">
+      <c r="L14" s="2" t="n">
         <v>44785</v>
       </c>
     </row>
@@ -845,24 +1021,36 @@
       <c r="B15" t="n">
         <v>13</v>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" t="n">
+        <v>13</v>
+      </c>
+      <c r="D15" t="n">
+        <v>13</v>
+      </c>
+      <c r="E15" t="n">
+        <v>13</v>
+      </c>
+      <c r="F15" t="n">
+        <v>13</v>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>Galletitas "9 de oro"</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="H15" t="n">
         <v>2</v>
       </c>
-      <c r="E15" t="n">
+      <c r="I15" t="n">
         <v>61.54</v>
       </c>
-      <c r="F15" t="n">
+      <c r="J15" t="n">
         <v>18.46</v>
       </c>
-      <c r="G15" t="n">
+      <c r="K15" t="n">
         <v>80</v>
       </c>
-      <c r="H15" s="2" t="n">
+      <c r="L15" s="2" t="n">
         <v>44988</v>
       </c>
     </row>
@@ -873,24 +1061,36 @@
       <c r="B16" t="n">
         <v>14</v>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" t="n">
+        <v>14</v>
+      </c>
+      <c r="E16" t="n">
+        <v>14</v>
+      </c>
+      <c r="F16" t="n">
+        <v>14</v>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>Galletitas "Don Satur"</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="H16" t="n">
         <v>3</v>
       </c>
-      <c r="E16" t="n">
+      <c r="I16" t="n">
         <v>53.85</v>
       </c>
-      <c r="F16" t="n">
+      <c r="J16" t="n">
         <v>16.15</v>
       </c>
-      <c r="G16" t="n">
+      <c r="K16" t="n">
         <v>70</v>
       </c>
-      <c r="H16" s="2" t="n">
+      <c r="L16" s="2" t="n">
         <v>45112</v>
       </c>
     </row>
@@ -901,24 +1101,36 @@
       <c r="B17" t="n">
         <v>15</v>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" t="n">
+        <v>15</v>
+      </c>
+      <c r="E17" t="n">
+        <v>15</v>
+      </c>
+      <c r="F17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>Gelatina "Bárbara"</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="H17" t="n">
         <v>5</v>
       </c>
-      <c r="E17" t="n">
+      <c r="I17" t="n">
         <v>53.85</v>
       </c>
-      <c r="F17" t="n">
+      <c r="J17" t="n">
         <v>16.15</v>
       </c>
-      <c r="G17" t="n">
+      <c r="K17" t="n">
         <v>70</v>
       </c>
-      <c r="H17" s="2" t="n">
+      <c r="L17" s="2" t="n">
         <v>45050</v>
       </c>
     </row>
@@ -929,24 +1141,36 @@
       <c r="B18" t="n">
         <v>16</v>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" t="n">
+        <v>16</v>
+      </c>
+      <c r="D18" t="n">
+        <v>16</v>
+      </c>
+      <c r="E18" t="n">
+        <v>16</v>
+      </c>
+      <c r="F18" t="n">
+        <v>16</v>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>Fideos "308"</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="H18" t="n">
         <v>8</v>
       </c>
-      <c r="E18" t="n">
+      <c r="I18" t="n">
         <v>46.15</v>
       </c>
-      <c r="F18" t="n">
+      <c r="J18" t="n">
         <v>13.85</v>
       </c>
-      <c r="G18" t="n">
+      <c r="K18" t="n">
         <v>60</v>
       </c>
-      <c r="H18" s="2" t="n">
+      <c r="L18" s="2" t="n">
         <v>45337</v>
       </c>
     </row>
@@ -957,24 +1181,36 @@
       <c r="B19" t="n">
         <v>17</v>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+      <c r="D19" t="n">
+        <v>17</v>
+      </c>
+      <c r="E19" t="n">
+        <v>17</v>
+      </c>
+      <c r="F19" t="n">
+        <v>17</v>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>Arvejas "Molto"</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="H19" t="n">
         <v>2</v>
       </c>
-      <c r="E19" t="n">
+      <c r="I19" t="n">
         <v>38.46</v>
       </c>
-      <c r="F19" t="n">
+      <c r="J19" t="n">
         <v>11.54</v>
       </c>
-      <c r="G19" t="n">
+      <c r="K19" t="n">
         <v>50</v>
       </c>
-      <c r="H19" s="2" t="n">
+      <c r="L19" s="2" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -985,24 +1221,36 @@
       <c r="B20" t="n">
         <v>18</v>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" t="n">
+        <v>18</v>
+      </c>
+      <c r="D20" t="n">
+        <v>18</v>
+      </c>
+      <c r="E20" t="n">
+        <v>18</v>
+      </c>
+      <c r="F20" t="n">
+        <v>18</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>Caldito "Knorr"</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="H20" t="n">
         <v>60</v>
       </c>
-      <c r="E20" t="n">
+      <c r="I20" t="n">
         <v>7.69</v>
       </c>
-      <c r="F20" t="n">
+      <c r="J20" t="n">
         <v>2.31</v>
       </c>
-      <c r="G20" t="n">
+      <c r="K20" t="n">
         <v>10</v>
       </c>
-      <c r="H20" s="2" t="n">
+      <c r="L20" s="2" t="n">
         <v>45427</v>
       </c>
     </row>
@@ -1013,24 +1261,36 @@
       <c r="B21" t="n">
         <v>19</v>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" t="n">
+        <v>19</v>
+      </c>
+      <c r="D21" t="n">
+        <v>19</v>
+      </c>
+      <c r="E21" t="n">
+        <v>19</v>
+      </c>
+      <c r="F21" t="n">
+        <v>19</v>
+      </c>
+      <c r="G21" t="inlineStr">
         <is>
           <t>Flan "Bárbara"</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="H21" t="n">
         <v>1</v>
       </c>
-      <c r="E21" t="n">
+      <c r="I21" t="n">
         <v>30.77</v>
       </c>
-      <c r="F21" t="n">
+      <c r="J21" t="n">
         <v>9.23</v>
       </c>
-      <c r="G21" t="n">
+      <c r="K21" t="n">
         <v>40</v>
       </c>
-      <c r="H21" s="2" t="n">
+      <c r="L21" s="2" t="n">
         <v>44908</v>
       </c>
     </row>
@@ -1041,24 +1301,36 @@
       <c r="B22" t="n">
         <v>20</v>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" t="n">
+        <v>20</v>
+      </c>
+      <c r="E22" t="n">
+        <v>20</v>
+      </c>
+      <c r="F22" t="n">
+        <v>20</v>
+      </c>
+      <c r="G22" t="inlineStr">
         <is>
           <t>Saborizante "Alicante"</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="H22" t="n">
         <v>24</v>
       </c>
-      <c r="E22" t="n">
+      <c r="I22" t="n">
         <v>23.08</v>
       </c>
-      <c r="F22" t="n">
+      <c r="J22" t="n">
         <v>6.920000000000002</v>
       </c>
-      <c r="G22" t="n">
+      <c r="K22" t="n">
         <v>30</v>
       </c>
-      <c r="H22" s="2" t="n">
+      <c r="L22" s="2" t="n">
         <v>44818</v>
       </c>
     </row>
@@ -1069,24 +1341,36 @@
       <c r="B23" t="n">
         <v>21</v>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" t="n">
+        <v>21</v>
+      </c>
+      <c r="D23" t="n">
+        <v>21</v>
+      </c>
+      <c r="E23" t="n">
+        <v>21</v>
+      </c>
+      <c r="F23" t="n">
+        <v>21</v>
+      </c>
+      <c r="G23" t="inlineStr">
         <is>
           <t>Maquina de afeitar "Gillette"</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="H23" t="n">
         <v>9</v>
       </c>
-      <c r="E23" t="n">
+      <c r="I23" t="n">
         <v>84.62</v>
       </c>
-      <c r="F23" t="n">
+      <c r="J23" t="n">
         <v>25.38</v>
       </c>
-      <c r="G23" t="n">
+      <c r="K23" t="n">
         <v>110</v>
       </c>
-      <c r="H23" s="2" t="n">
+      <c r="L23" s="2" t="n">
         <v>45023</v>
       </c>
     </row>
@@ -1097,24 +1381,36 @@
       <c r="B24" t="n">
         <v>22</v>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" t="n">
+        <v>22</v>
+      </c>
+      <c r="D24" t="n">
+        <v>22</v>
+      </c>
+      <c r="E24" t="n">
+        <v>22</v>
+      </c>
+      <c r="F24" t="n">
+        <v>22</v>
+      </c>
+      <c r="G24" t="inlineStr">
         <is>
           <t>Tostadas "Manieri"</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="H24" t="n">
         <v>2</v>
       </c>
-      <c r="E24" t="n">
+      <c r="I24" t="n">
         <v>69.23</v>
       </c>
-      <c r="F24" t="n">
+      <c r="J24" t="n">
         <v>20.77</v>
       </c>
-      <c r="G24" t="n">
+      <c r="K24" t="n">
         <v>90</v>
       </c>
-      <c r="H24" s="2" t="n">
+      <c r="L24" s="2" t="n">
         <v>44998</v>
       </c>
     </row>
@@ -1125,24 +1421,36 @@
       <c r="B25" t="n">
         <v>23</v>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" t="n">
+        <v>23</v>
+      </c>
+      <c r="D25" t="n">
+        <v>23</v>
+      </c>
+      <c r="E25" t="n">
+        <v>23</v>
+      </c>
+      <c r="F25" t="n">
+        <v>23</v>
+      </c>
+      <c r="G25" t="inlineStr">
         <is>
           <t>Galletitas "Hojalmar"</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="H25" t="n">
         <v>4</v>
       </c>
-      <c r="E25" t="n">
+      <c r="I25" t="n">
         <v>46.16</v>
       </c>
-      <c r="F25" t="n">
+      <c r="J25" t="n">
         <v>13.84</v>
       </c>
-      <c r="G25" t="n">
+      <c r="K25" t="n">
         <v>60</v>
       </c>
-      <c r="H25" s="2" t="n">
+      <c r="L25" s="2" t="n">
         <v>44874</v>
       </c>
     </row>
@@ -1153,24 +1461,36 @@
       <c r="B26" t="n">
         <v>24</v>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" t="n">
+        <v>24</v>
+      </c>
+      <c r="D26" t="n">
+        <v>24</v>
+      </c>
+      <c r="E26" t="n">
+        <v>24</v>
+      </c>
+      <c r="F26" t="n">
+        <v>24</v>
+      </c>
+      <c r="G26" t="inlineStr">
         <is>
           <t>Galletitas pepas "Cilo"</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="H26" t="n">
         <v>2</v>
       </c>
-      <c r="E26" t="n">
+      <c r="I26" t="n">
         <v>92.31</v>
       </c>
-      <c r="F26" t="n">
+      <c r="J26" t="n">
         <v>27.69</v>
       </c>
-      <c r="G26" t="n">
+      <c r="K26" t="n">
         <v>120</v>
       </c>
-      <c r="H26" s="2" t="n">
+      <c r="L26" s="2" t="n">
         <v>44785</v>
       </c>
     </row>
@@ -1181,24 +1501,36 @@
       <c r="B27" t="n">
         <v>25</v>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" t="n">
+        <v>25</v>
+      </c>
+      <c r="D27" t="n">
+        <v>25</v>
+      </c>
+      <c r="E27" t="n">
+        <v>25</v>
+      </c>
+      <c r="F27" t="n">
+        <v>25</v>
+      </c>
+      <c r="G27" t="inlineStr">
         <is>
           <t>Galletitas "Lenguitas" coco</t>
         </is>
       </c>
-      <c r="D27" t="n">
+      <c r="H27" t="n">
         <v>3</v>
       </c>
-      <c r="E27" t="n">
+      <c r="I27" t="n">
         <v>100</v>
       </c>
-      <c r="F27" t="n">
+      <c r="J27" t="n">
         <v>30</v>
       </c>
-      <c r="G27" t="n">
+      <c r="K27" t="n">
         <v>130</v>
       </c>
-      <c r="H27" s="2" t="n">
+      <c r="L27" s="2" t="n">
         <v>44988</v>
       </c>
     </row>
@@ -1209,24 +1541,36 @@
       <c r="B28" t="n">
         <v>26</v>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" t="n">
+        <v>26</v>
+      </c>
+      <c r="D28" t="n">
+        <v>26</v>
+      </c>
+      <c r="E28" t="n">
+        <v>26</v>
+      </c>
+      <c r="F28" t="n">
+        <v>26</v>
+      </c>
+      <c r="G28" t="inlineStr">
         <is>
           <t>Galletitas "9 de oro"</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="H28" t="n">
         <v>1</v>
       </c>
-      <c r="E28" t="n">
+      <c r="I28" t="n">
         <v>53.85</v>
       </c>
-      <c r="F28" t="n">
+      <c r="J28" t="n">
         <v>16.15</v>
       </c>
-      <c r="G28" t="n">
+      <c r="K28" t="n">
         <v>70</v>
       </c>
-      <c r="H28" s="2" t="n">
+      <c r="L28" s="2" t="n">
         <v>45112</v>
       </c>
     </row>
@@ -1237,24 +1581,36 @@
       <c r="B29" t="n">
         <v>27</v>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" t="n">
+        <v>27</v>
+      </c>
+      <c r="D29" t="n">
+        <v>27</v>
+      </c>
+      <c r="E29" t="n">
+        <v>27</v>
+      </c>
+      <c r="F29" t="n">
+        <v>27</v>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>Pan rallado</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="H29" t="n">
         <v>2</v>
       </c>
-      <c r="E29" t="n">
+      <c r="I29" t="n">
         <v>61.54</v>
       </c>
-      <c r="F29" t="n">
+      <c r="J29" t="n">
         <v>18.46</v>
       </c>
-      <c r="G29" t="n">
+      <c r="K29" t="n">
         <v>80</v>
       </c>
-      <c r="H29" s="2" t="n">
+      <c r="L29" s="2" t="n">
         <v>45050</v>
       </c>
     </row>
@@ -1265,24 +1621,36 @@
       <c r="B30" t="n">
         <v>28</v>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" t="n">
+        <v>28</v>
+      </c>
+      <c r="D30" t="n">
+        <v>28</v>
+      </c>
+      <c r="E30" t="n">
+        <v>28</v>
+      </c>
+      <c r="F30" t="n">
+        <v>28</v>
+      </c>
+      <c r="G30" t="inlineStr">
         <is>
           <t>Fideos "Sol pampero"</t>
         </is>
       </c>
-      <c r="D30" t="n">
+      <c r="H30" t="n">
         <v>3</v>
       </c>
-      <c r="E30" t="n">
+      <c r="I30" t="n">
         <v>46.15</v>
       </c>
-      <c r="F30" t="n">
+      <c r="J30" t="n">
         <v>13.85</v>
       </c>
-      <c r="G30" t="n">
+      <c r="K30" t="n">
         <v>60</v>
       </c>
-      <c r="H30" s="2" t="n">
+      <c r="L30" s="2" t="n">
         <v>45337</v>
       </c>
     </row>
@@ -1293,24 +1661,36 @@
       <c r="B31" t="n">
         <v>29</v>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" t="n">
+        <v>29</v>
+      </c>
+      <c r="D31" t="n">
+        <v>29</v>
+      </c>
+      <c r="E31" t="n">
+        <v>29</v>
+      </c>
+      <c r="F31" t="n">
+        <v>29</v>
+      </c>
+      <c r="G31" t="inlineStr">
         <is>
           <t>Arroz "San Salvador"  1kg.</t>
         </is>
       </c>
-      <c r="D31" t="n">
+      <c r="H31" t="n">
         <v>4</v>
       </c>
-      <c r="E31" t="n">
+      <c r="I31" t="n">
         <v>84.62</v>
       </c>
-      <c r="F31" t="n">
+      <c r="J31" t="n">
         <v>25.38</v>
       </c>
-      <c r="G31" t="n">
+      <c r="K31" t="n">
         <v>110</v>
       </c>
-      <c r="H31" s="2" t="n">
+      <c r="L31" s="2" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -1321,24 +1701,36 @@
       <c r="B32" t="n">
         <v>30</v>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" t="n">
+        <v>30</v>
+      </c>
+      <c r="D32" t="n">
+        <v>30</v>
+      </c>
+      <c r="E32" t="n">
+        <v>30</v>
+      </c>
+      <c r="F32" t="n">
+        <v>30</v>
+      </c>
+      <c r="G32" t="inlineStr">
         <is>
           <t>Nuevo producto</t>
         </is>
       </c>
-      <c r="D32" t="n">
-        <v>10</v>
-      </c>
-      <c r="E32" t="n">
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
         <v>5</v>
       </c>
-      <c r="F32" t="n">
+      <c r="J32" t="n">
         <v>7</v>
       </c>
-      <c r="G32" t="n">
+      <c r="K32" t="n">
         <v>12</v>
       </c>
-      <c r="H32" s="2" t="n">
+      <c r="L32" s="2" t="n">
         <v>44907</v>
       </c>
     </row>

</xml_diff>